<commit_message>
Draw Select tile, [Fixed] Flip & Rotate tile
</commit_message>
<xml_diff>
--- a/Doc/วิธีคำนวณ Tile Position.xlsx
+++ b/Doc/วิธีคำนวณ Tile Position.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>180 degree</t>
   </si>
@@ -47,10 +47,13 @@
     <t>ค่าเริ่มต้น Rotate</t>
   </si>
   <si>
-    <t>270 Degree Flip Horizontal</t>
-  </si>
-  <si>
     <t>180 Degree Flip Horizontal</t>
+  </si>
+  <si>
+    <t>Horizontal เริ่มที่ค่า</t>
+  </si>
+  <si>
+    <t>270 Degree Flip Vertical</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,6 +443,9 @@
       <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
@@ -451,6 +457,9 @@
       <c r="C2" s="2">
         <v>5</v>
       </c>
+      <c r="D2" s="2">
+        <v>2147483648</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -490,7 +499,7 @@
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <f>B2+C2+B2</f>
@@ -501,7 +510,7 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <f>B2+C2+B2+A2</f>

</xml_diff>